<commit_message>
Fix defect: change name of field comment_id -> pcomment_id
</commit_message>
<xml_diff>
--- a/doc/backend/db/TRN-MiniBlog_DatabaseDesign_TRILE.xlsx
+++ b/doc/backend/db/TRN-MiniBlog_DatabaseDesign_TRILE.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="34560" windowHeight="17020" tabRatio="818" activeTab="3"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="34560" windowHeight="17020" tabRatio="818"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="11" r:id="rId1"/>
@@ -138,7 +138,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="192">
   <si>
     <t>No</t>
   </si>
@@ -678,9 +678,6 @@
     <t>post_id</t>
   </si>
   <si>
-    <t>CommenttID</t>
-  </si>
-  <si>
     <t>comment_id</t>
   </si>
   <si>
@@ -709,6 +706,18 @@
   </si>
   <si>
     <t>user</t>
+  </si>
+  <si>
+    <t>PCommenttID</t>
+  </si>
+  <si>
+    <t>pcomment_id</t>
+  </si>
+  <si>
+    <t>1.0.1</t>
+  </si>
+  <si>
+    <t>Change name of field comment_id -&gt; pcomment_id</t>
   </si>
 </sst>
 </file>
@@ -2005,7 +2014,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="532">
+  <cellStyleXfs count="533">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2025,6 +2034,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -4338,7 +4350,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="532">
+  <cellStyles count="533">
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
@@ -4863,6 +4875,7 @@
     <cellStyle name="Followed Hyperlink" xfId="529" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="530" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="531" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="532" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="ハイパーリンク 2" xfId="4"/>
@@ -5443,7 +5456,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AZ35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="O13" sqref="O13:AK14"/>
     </sheetView>
   </sheetViews>
@@ -8016,7 +8029,7 @@
   <dimension ref="B1:F34"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="11" x14ac:dyDescent="0"/>
@@ -8066,10 +8079,18 @@
       <c r="F3" s="96"/>
     </row>
     <row r="4" spans="2:6">
-      <c r="B4" s="97"/>
-      <c r="C4" s="115"/>
-      <c r="D4" s="98"/>
-      <c r="E4" s="99"/>
+      <c r="B4" s="97">
+        <v>42062</v>
+      </c>
+      <c r="C4" s="115" t="s">
+        <v>190</v>
+      </c>
+      <c r="D4" s="98" t="s">
+        <v>114</v>
+      </c>
+      <c r="E4" s="99" t="s">
+        <v>191</v>
+      </c>
       <c r="F4" s="100"/>
     </row>
     <row r="5" spans="2:6">
@@ -8585,7 +8606,7 @@
   </sheetPr>
   <dimension ref="A1:O39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
@@ -8930,7 +8951,7 @@
         <v>126</v>
       </c>
       <c r="D19" s="129" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E19" s="66" t="s">
         <v>3</v>
@@ -9404,7 +9425,7 @@
         <v>141</v>
       </c>
       <c r="N13" s="170" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="O13" s="171" t="s">
         <v>130</v>
@@ -9465,13 +9486,13 @@
         <v>2</v>
       </c>
       <c r="B15" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="C15" s="18" t="s">
         <v>181</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="D15" s="65" t="s">
         <v>182</v>
-      </c>
-      <c r="D15" s="65" t="s">
-        <v>183</v>
       </c>
       <c r="E15" s="201" t="s">
         <v>3</v>
@@ -9513,7 +9534,7 @@
         <v>143</v>
       </c>
       <c r="D16" s="65" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E16" s="66" t="s">
         <v>3</v>
@@ -9589,10 +9610,10 @@
         <v>7</v>
       </c>
       <c r="B20" s="63" t="s">
+        <v>183</v>
+      </c>
+      <c r="C20" s="65" t="s">
         <v>184</v>
-      </c>
-      <c r="C20" s="65" t="s">
-        <v>185</v>
       </c>
       <c r="D20" s="65" t="s">
         <v>127</v>
@@ -9854,7 +9875,7 @@
   <dimension ref="A1:T39"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+      <selection activeCell="F5" sqref="F5:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="11" x14ac:dyDescent="0"/>
@@ -9921,7 +9942,9 @@
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="214"/>
+      <c r="F4" s="217">
+        <v>42062</v>
+      </c>
       <c r="G4" s="218"/>
     </row>
     <row r="5" spans="1:20" ht="13">
@@ -10028,7 +10051,7 @@
         <v>177</v>
       </c>
       <c r="N13" s="198" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="O13" s="162" t="s">
         <v>130</v>
@@ -10193,10 +10216,10 @@
         <v>6</v>
       </c>
       <c r="B19" s="63" t="s">
-        <v>178</v>
+        <v>188</v>
       </c>
       <c r="C19" s="65" t="s">
-        <v>179</v>
+        <v>189</v>
       </c>
       <c r="D19" s="65" t="s">
         <v>53</v>
@@ -10206,7 +10229,7 @@
       </c>
       <c r="F19" s="67"/>
       <c r="G19" s="106" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -10384,7 +10407,7 @@
       </c>
       <c r="D33" s="207"/>
       <c r="E33" s="206" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F33" s="207"/>
       <c r="G33" s="159" t="s">
@@ -10415,10 +10438,10 @@
         <v>3</v>
       </c>
       <c r="B35" s="45" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C35" s="210" t="s">
-        <v>179</v>
+        <v>189</v>
       </c>
       <c r="D35" s="211"/>
       <c r="E35" s="210" t="s">

</xml_diff>